<commit_message>
Added endpoint to api
</commit_message>
<xml_diff>
--- a/srv/backend/birds_data.xlsx
+++ b/srv/backend/birds_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PM34NO\PycharmProjects\bird-site\srv\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C98049EA-FBB8-4B5F-B3F9-4960EAC85AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F1CC89-53A6-40DB-9825-52B4A0C701E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="2" r:id="rId1"/>
@@ -1105,7 +1105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4FDEAF-0B66-4E2C-AFD6-77F4207E41CF}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1334,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147B6A7F-2A5C-40EF-9F6C-7D7A350D77D2}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1360,11 +1360,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6240EFE-CA97-4B5E-9E1A-7A3648DFCC35}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1923,7 +1926,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>